<commit_message>
Add errors to part B
</commit_message>
<xml_diff>
--- a/מתנד הרמוני.xlsx
+++ b/מתנד הרמוני.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TLP-001\Documents\MATLAB\Lab2A-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F40AE65-0F53-4FDE-9F0D-BDE8EE5CB37A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D840C70-A524-4636-B73E-CAB5FF878768}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{971A0516-501A-45D9-A5C8-9A13949A1454}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="2" xr2:uid="{971A0516-501A-45D9-A5C8-9A13949A1454}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1130,10 +1130,10 @@
                   <c:v>35.714285714285715</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.372881355932201</c:v>
+                  <c:v>42.372881355932208</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47.393364928909946</c:v>
+                  <c:v>47.393364928909953</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>45.871559633027523</c:v>
@@ -5789,8 +5789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D473B3A5-D74E-4E30-A305-E9ED45771281}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5840,7 +5840,7 @@
         <v>3.1334800000000001E-3</v>
       </c>
       <c r="G2">
-        <f>2*B2/F2</f>
+        <f>1/E2</f>
         <v>16.129032258064516</v>
       </c>
     </row>
@@ -5866,7 +5866,7 @@
         <v>3.9094200000000003E-3</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G10" si="2">2*B3/F3</f>
+        <f t="shared" ref="G3:G10" si="2">1/E3</f>
         <v>18.018018018018019</v>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>42.372881355932201</v>
+        <v>42.372881355932208</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>47.393364928909946</v>
+        <v>47.393364928909953</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -6063,8 +6063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6A29C7-B872-4D59-912E-5AD023568170}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>